<commit_message>
Updated Gwent stats and small changes to Kinde PW Dashboard (first post)
</commit_message>
<xml_diff>
--- a/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
+++ b/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>season</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>M2_08 Draconid 2020</t>
+  </si>
+  <si>
+    <t>M2_09 Dryad 2020</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -641,7 +644,7 @@
         <v>10546</v>
       </c>
       <c r="E9">
-        <v>838672</v>
+        <v>838212</v>
       </c>
       <c r="F9">
         <v>9946</v>
@@ -651,6 +654,32 @@
       </c>
       <c r="H9">
         <v>10246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>9678</v>
+      </c>
+      <c r="D10">
+        <v>10725</v>
+      </c>
+      <c r="E10">
+        <v>855528</v>
+      </c>
+      <c r="F10">
+        <v>9946</v>
+      </c>
+      <c r="G10">
+        <v>10046</v>
+      </c>
+      <c r="H10">
+        <v>10183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added link to article on TBG and updated Gwent Stats
</commit_message>
<xml_diff>
--- a/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
+++ b/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>season</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>M2_09 Dryad 2020</t>
+  </si>
+  <si>
+    <t>M2_10 Cat 2020</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -670,7 +673,7 @@
         <v>10725</v>
       </c>
       <c r="E10">
-        <v>855528</v>
+        <v>854877</v>
       </c>
       <c r="F10">
         <v>9946</v>
@@ -680,6 +683,32 @@
       </c>
       <c r="H10">
         <v>10183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>9703</v>
+      </c>
+      <c r="D11">
+        <v>10804</v>
+      </c>
+      <c r="E11">
+        <v>929613</v>
+      </c>
+      <c r="F11">
+        <v>9977</v>
+      </c>
+      <c r="G11">
+        <v>10067</v>
+      </c>
+      <c r="H11">
+        <v>10176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated gwent masters 2 data
</commit_message>
<xml_diff>
--- a/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
+++ b/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>season</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>M2_10 Cat 2020</t>
+  </si>
+  <si>
+    <t>M2_11 Mahakam 2020</t>
+  </si>
+  <si>
+    <t>M2_12 Wild Hunt 2020</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,7 +497,7 @@
         <v>10537</v>
       </c>
       <c r="E3">
-        <v>769358</v>
+        <v>769172</v>
       </c>
       <c r="F3">
         <v>9832</v>
@@ -517,7 +523,7 @@
         <v>10669</v>
       </c>
       <c r="E4">
-        <v>862678</v>
+        <v>862283</v>
       </c>
       <c r="F4">
         <v>9867</v>
@@ -543,7 +549,7 @@
         <v>10751</v>
       </c>
       <c r="E5">
-        <v>1004830</v>
+        <v>1004603</v>
       </c>
       <c r="F5">
         <v>9952</v>
@@ -595,7 +601,7 @@
         <v>10597</v>
       </c>
       <c r="E7">
-        <v>793401</v>
+        <v>793013</v>
       </c>
       <c r="F7">
         <v>9896</v>
@@ -621,7 +627,7 @@
         <v>10667</v>
       </c>
       <c r="E8">
-        <v>996742</v>
+        <v>996516</v>
       </c>
       <c r="F8">
         <v>9978</v>
@@ -647,7 +653,7 @@
         <v>10546</v>
       </c>
       <c r="E9">
-        <v>838212</v>
+        <v>837545</v>
       </c>
       <c r="F9">
         <v>9946</v>
@@ -673,7 +679,7 @@
         <v>10725</v>
       </c>
       <c r="E10">
-        <v>854877</v>
+        <v>854593</v>
       </c>
       <c r="F10">
         <v>9946</v>
@@ -699,7 +705,7 @@
         <v>10804</v>
       </c>
       <c r="E11">
-        <v>929613</v>
+        <v>928845</v>
       </c>
       <c r="F11">
         <v>9977</v>
@@ -709,6 +715,58 @@
       </c>
       <c r="H11">
         <v>10176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>9706</v>
+      </c>
+      <c r="D12">
+        <v>10783</v>
+      </c>
+      <c r="E12">
+        <v>983150</v>
+      </c>
+      <c r="F12">
+        <v>10000</v>
+      </c>
+      <c r="G12">
+        <v>10090</v>
+      </c>
+      <c r="H12">
+        <v>10216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>9756</v>
+      </c>
+      <c r="D13">
+        <v>10724</v>
+      </c>
+      <c r="E13">
+        <v>1182983</v>
+      </c>
+      <c r="F13">
+        <v>10070</v>
+      </c>
+      <c r="G13">
+        <v>10172</v>
+      </c>
+      <c r="H13">
+        <v>10313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Gwent Pro Rank data
</commit_message>
<xml_diff>
--- a/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
+++ b/assets/posts/2020-09-01-GwentProRankAnalysis/seasonal_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>season</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>M2_12 Wild Hunt 2020</t>
+  </si>
+  <si>
+    <t>M3_01 Wolf 2021</t>
+  </si>
+  <si>
+    <t>M3_02 Love 2021</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -757,7 +763,7 @@
         <v>10724</v>
       </c>
       <c r="E13">
-        <v>1182983</v>
+        <v>1182353</v>
       </c>
       <c r="F13">
         <v>10070</v>
@@ -767,6 +773,58 @@
       </c>
       <c r="H13">
         <v>10313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>9637</v>
+      </c>
+      <c r="D14">
+        <v>10653</v>
+      </c>
+      <c r="E14">
+        <v>808651</v>
+      </c>
+      <c r="F14">
+        <v>9916</v>
+      </c>
+      <c r="G14">
+        <v>10044</v>
+      </c>
+      <c r="H14">
+        <v>10295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>9684</v>
+      </c>
+      <c r="D15">
+        <v>10714</v>
+      </c>
+      <c r="E15">
+        <v>917491</v>
+      </c>
+      <c r="F15">
+        <v>9975</v>
+      </c>
+      <c r="G15">
+        <v>10097</v>
+      </c>
+      <c r="H15">
+        <v>10325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>